<commit_message>
Added DNI to value
</commit_message>
<xml_diff>
--- a/Boards/Main_Board/_WWW/Bill_of_Materials.xlsx
+++ b/Boards/Main_Board/_WWW/Bill_of_Materials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\f2022\ECE_4440\Git\Capstone-Electrical\Boards\Main_Board\_WWW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EJ\Capstone\Capstone-Electrical\Boards\Main_Board\_WWW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815376CA-ABEF-485F-8715-322E405D8062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475B40F7-2B88-4DF5-886E-31B776E17E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4230" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="127">
   <si>
     <t>100 uF</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>REV 21</t>
+  </si>
+  <si>
+    <t>DNI</t>
   </si>
 </sst>
 </file>
@@ -797,18 +800,18 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -818,7 +821,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>125</v>
       </c>
@@ -828,7 +831,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -836,7 +839,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -856,7 +859,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -876,7 +879,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -896,7 +899,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -916,7 +919,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -936,7 +939,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -956,7 +959,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -976,7 +979,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -994,7 +997,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -1112,7 +1115,9 @@
       <c r="C18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1120,7 +1125,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -1130,7 +1135,9 @@
       <c r="C19" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1138,7 +1145,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -1148,7 +1155,9 @@
       <c r="C20" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>19</v>
       </c>
@@ -1156,7 +1165,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -1166,7 +1175,9 @@
       <c r="C21" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1174,7 +1185,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -1184,7 +1195,9 @@
       <c r="C22" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1192,7 +1205,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -1202,7 +1215,9 @@
       <c r="C23" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1210,7 +1225,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -1220,7 +1235,9 @@
       <c r="C24" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1228,7 +1245,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -1248,7 +1265,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -1268,7 +1285,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -1286,7 +1303,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -1306,7 +1323,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -1326,7 +1343,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -1346,7 +1363,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -1366,7 +1383,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -1382,7 +1399,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -1402,7 +1419,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -1422,7 +1439,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>31</v>
       </c>
@@ -1442,7 +1459,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>32</v>
       </c>
@@ -1462,7 +1479,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>33</v>
       </c>
@@ -1482,7 +1499,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>34</v>
       </c>
@@ -1502,7 +1519,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>35</v>
       </c>
@@ -1518,7 +1535,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>36</v>
       </c>
@@ -1536,7 +1553,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>37</v>
       </c>
@@ -1546,7 +1563,9 @@
       <c r="C41" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D41" s="5"/>
+      <c r="D41" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E41" s="5">
         <v>5010</v>
       </c>
@@ -1554,7 +1573,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>38</v>
       </c>
@@ -1572,7 +1591,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>39</v>
       </c>
@@ -1590,7 +1609,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>40</v>
       </c>
@@ -1608,7 +1627,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>41</v>
       </c>
@@ -1626,7 +1645,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>42</v>
       </c>

</xml_diff>